<commit_message>
solved 15650, 15651, 15652, 15654
</commit_message>
<xml_diff>
--- a/study_algo_record_date.xlsx
+++ b/study_algo_record_date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prepare-coding-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2130D96B-4E81-4376-9CE2-DB77C104058F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15319DFA-2A4F-4808-B066-7270FE277E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{142D3439-D715-4BB9-B0EC-A88EA240EC91}"/>
   </bookViews>
@@ -1784,7 +1784,7 @@
   <dimension ref="A1:S86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2025,7 +2025,9 @@
       <c r="G18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="4"/>
+      <c r="H18" s="27">
+        <v>44533</v>
+      </c>
       <c r="J18" s="2">
         <v>1759</v>
       </c>
@@ -2050,7 +2052,9 @@
       <c r="G19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="4"/>
+      <c r="H19" s="27">
+        <v>44533</v>
+      </c>
       <c r="J19" s="2">
         <v>14501</v>
       </c>
@@ -2075,7 +2079,9 @@
       <c r="G20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="4"/>
+      <c r="H20" s="27">
+        <v>44533</v>
+      </c>
       <c r="J20" s="2">
         <v>14889</v>
       </c>
@@ -2100,7 +2106,9 @@
       <c r="G21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="4"/>
+      <c r="H21" s="27">
+        <v>44533</v>
+      </c>
       <c r="J21" s="2">
         <v>15661</v>
       </c>

</xml_diff>

<commit_message>
solved 15655, 15656, 15657
</commit_message>
<xml_diff>
--- a/study_algo_record_date.xlsx
+++ b/study_algo_record_date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prepare-coding-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15319DFA-2A4F-4808-B066-7270FE277E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECEDC65-1067-45E3-948A-F84368F35768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{142D3439-D715-4BB9-B0EC-A88EA240EC91}"/>
   </bookViews>
@@ -1784,7 +1784,7 @@
   <dimension ref="A1:S86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2136,7 +2136,9 @@
       <c r="G22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="4"/>
+      <c r="H22" s="27">
+        <v>44534</v>
+      </c>
       <c r="J22" s="2">
         <v>2529</v>
       </c>
@@ -2164,7 +2166,9 @@
       <c r="G23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="4"/>
+      <c r="H23" s="27">
+        <v>44534</v>
+      </c>
       <c r="J23" s="2">
         <v>1248</v>
       </c>
@@ -2186,7 +2190,9 @@
       <c r="G24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="27">
+        <v>44534</v>
+      </c>
       <c r="J24" s="6"/>
       <c r="K24" s="7"/>
       <c r="L24" s="5"/>

</xml_diff>